<commit_message>
"need to update items from MSA data"
</commit_message>
<xml_diff>
--- a/data_dictionary.xlsx
+++ b/data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\mgsc410\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FC521E8-A884-4163-8FC2-2EF659FC3899}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE15C97-7936-43D7-809B-134897256473}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1F7D180B-2BA4-4832-A9A8-DAB502E467AA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1F7D180B-2BA4-4832-A9A8-DAB502E467AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="76">
   <si>
     <t>Term</t>
   </si>
@@ -75,9 +74,6 @@
     <t>weekly_sales</t>
   </si>
   <si>
-    <t>double</t>
-  </si>
-  <si>
     <t>isHoliday</t>
   </si>
   <si>
@@ -139,6 +135,129 @@
   </si>
   <si>
     <t>dma</t>
+  </si>
+  <si>
+    <t>DMA</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>DMA Name</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Population 18+</t>
+  </si>
+  <si>
+    <t>Household Count</t>
+  </si>
+  <si>
+    <t>Med HHld Income</t>
+  </si>
+  <si>
+    <t>HHlds No Vehicles</t>
+  </si>
+  <si>
+    <t>HHlds 1-2 Vehicles</t>
+  </si>
+  <si>
+    <t>HHlds 2+ Vehicles</t>
+  </si>
+  <si>
+    <t>HHld Exp - Public Transport</t>
+  </si>
+  <si>
+    <t>HHld Exp - Intercity Bus Fare</t>
+  </si>
+  <si>
+    <t>HHld Exp - Mass Transit</t>
+  </si>
+  <si>
+    <t>HHld Exp - Taxi</t>
+  </si>
+  <si>
+    <t>HHld Exp - Other Public Transportation</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>African American</t>
+  </si>
+  <si>
+    <t>American Indian</t>
+  </si>
+  <si>
+    <t>Asian</t>
+  </si>
+  <si>
+    <t>Hawaiian/Pacific Islander</t>
+  </si>
+  <si>
+    <t>Other Race</t>
+  </si>
+  <si>
+    <t>Multi-Race</t>
+  </si>
+  <si>
+    <t>Hispanic</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>Non-DMA Areas</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>"PI- 18803 DMAs.xlsx"</t>
+  </si>
+  <si>
+    <t>Lyft</t>
+  </si>
+  <si>
+    <t>"midwest.xlsx"</t>
+  </si>
+  <si>
+    <t>"northeast.xlsx"</t>
+  </si>
+  <si>
+    <t>"west.xlsx"</t>
+  </si>
+  <si>
+    <t>"south.xlsx"</t>
+  </si>
+  <si>
+    <t>MSA</t>
+  </si>
+  <si>
+    <t>Chicago</t>
+  </si>
+  <si>
+    <t>Source: Consumer Expenditure Survey, U.S. Bureau of Labor Statistics, September, 2018</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>Los Angeles</t>
+  </si>
+  <si>
+    <t>Baltimore</t>
   </si>
 </sst>
 </file>
@@ -502,21 +621,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81B2E13A-A86E-4147-9A8B-07F7836F86E0}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -539,7 +660,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -556,7 +677,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -573,7 +694,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -590,12 +711,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D5">
         <v>24924.5</v>
@@ -607,12 +728,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
@@ -624,7 +745,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -638,10 +759,10 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -655,15 +776,15 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D9">
         <v>42.31</v>
@@ -672,18 +793,18 @@
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D10">
         <v>2.5720000000000001</v>
@@ -692,15 +813,15 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D11">
         <v>211.0963582</v>
@@ -709,15 +830,15 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D12">
         <v>8.1059999999999999</v>
@@ -726,15 +847,15 @@
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
         <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -743,30 +864,30 @@
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -780,29 +901,29 @@
         <v>10</v>
       </c>
       <c r="F15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>27</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D16" t="s">
         <v>28</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>29</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>30</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
@@ -814,27 +935,537 @@
         <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" t="s">
-        <v>34</v>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>524050.67609000002</v>
+      </c>
+      <c r="E22" t="s">
+        <v>65</v>
+      </c>
+      <c r="F22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23">
+        <v>63.099780000000003</v>
+      </c>
+      <c r="E23" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <v>-151.23083</v>
+      </c>
+      <c r="E24" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" t="s">
+        <v>65</v>
+      </c>
+      <c r="F25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26">
+        <v>102531</v>
+      </c>
+      <c r="E26" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <v>48817</v>
+      </c>
+      <c r="E27" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28">
+        <v>68110</v>
+      </c>
+      <c r="E28" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29">
+        <v>11966</v>
+      </c>
+      <c r="E29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30">
+        <v>16091</v>
+      </c>
+      <c r="E30" t="s">
+        <v>65</v>
+      </c>
+      <c r="F30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31">
+        <v>20760</v>
+      </c>
+      <c r="E31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <v>748.84</v>
+      </c>
+      <c r="E32" t="s">
+        <v>65</v>
+      </c>
+      <c r="F32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>49</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33">
+        <v>22.13</v>
+      </c>
+      <c r="E33" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34">
+        <v>128.66</v>
+      </c>
+      <c r="E34" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35">
+        <v>28.71</v>
+      </c>
+      <c r="E35" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36">
+        <v>87.49</v>
+      </c>
+      <c r="E36" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37">
+        <v>57829</v>
+      </c>
+      <c r="E37" t="s">
+        <v>65</v>
+      </c>
+      <c r="F37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38">
+        <v>2118</v>
+      </c>
+      <c r="E38" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39">
+        <v>29940</v>
+      </c>
+      <c r="E39" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>56</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40">
+        <v>10488</v>
+      </c>
+      <c r="E40" t="s">
+        <v>65</v>
+      </c>
+      <c r="F40" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>57</v>
+      </c>
+      <c r="B41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41">
+        <v>364</v>
+      </c>
+      <c r="E41" t="s">
+        <v>65</v>
+      </c>
+      <c r="F41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>58</v>
+      </c>
+      <c r="B42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42">
+        <v>672</v>
+      </c>
+      <c r="E42" t="s">
+        <v>65</v>
+      </c>
+      <c r="F42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43">
+        <v>33247</v>
+      </c>
+      <c r="E43" t="s">
+        <v>65</v>
+      </c>
+      <c r="F43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44">
+        <v>7152</v>
+      </c>
+      <c r="E44" t="s">
+        <v>65</v>
+      </c>
+      <c r="F44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" t="s">
+        <v>71</v>
+      </c>
+      <c r="E45" t="s">
+        <v>72</v>
+      </c>
+      <c r="F45" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" t="s">
+        <v>73</v>
+      </c>
+      <c r="E46" t="s">
+        <v>72</v>
+      </c>
+      <c r="F46" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" t="s">
+        <v>74</v>
+      </c>
+      <c r="E47" t="s">
+        <v>72</v>
+      </c>
+      <c r="F47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" t="s">
+        <v>75</v>
+      </c>
+      <c r="E48" t="s">
+        <v>72</v>
+      </c>
+      <c r="F48" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all docs data desc done
</commit_message>
<xml_diff>
--- a/data_dictionary.xlsx
+++ b/data_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\mgsc410\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE15C97-7936-43D7-809B-134897256473}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC690D27-8C7A-4DA6-BEE7-D6D0AD75698B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1F7D180B-2BA4-4832-A9A8-DAB502E467AA}"/>
+    <workbookView xWindow="12456" yWindow="4272" windowWidth="17280" windowHeight="8964" xr2:uid="{1F7D180B-2BA4-4832-A9A8-DAB502E467AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="122">
   <si>
     <t>Term</t>
   </si>
@@ -258,12 +258,153 @@
   </si>
   <si>
     <t>Baltimore</t>
+  </si>
+  <si>
+    <t>num_consumer_units</t>
+  </si>
+  <si>
+    <t>income_before_taxes</t>
+  </si>
+  <si>
+    <t>int/string</t>
+  </si>
+  <si>
+    <t>age_of_ref_person</t>
+  </si>
+  <si>
+    <t>people</t>
+  </si>
+  <si>
+    <t>child_under_18</t>
+  </si>
+  <si>
+    <t>adult_over_65</t>
+  </si>
+  <si>
+    <t>earners</t>
+  </si>
+  <si>
+    <t>vehicles</t>
+  </si>
+  <si>
+    <t>perc_homeowner</t>
+  </si>
+  <si>
+    <t>avg_annual_expenditure</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>food_at_home</t>
+  </si>
+  <si>
+    <t>Cereals and bakery products</t>
+  </si>
+  <si>
+    <t>Meats, poultry, fish, and eggs</t>
+  </si>
+  <si>
+    <t>Dairy products</t>
+  </si>
+  <si>
+    <t>Fruits and vegetables</t>
+  </si>
+  <si>
+    <t>Other food at home</t>
+  </si>
+  <si>
+    <t>Food away from home</t>
+  </si>
+  <si>
+    <t>alcohol</t>
+  </si>
+  <si>
+    <t>Housing</t>
+  </si>
+  <si>
+    <t>Shelter</t>
+  </si>
+  <si>
+    <t>Owned dwellings</t>
+  </si>
+  <si>
+    <t>Rented dwellings</t>
+  </si>
+  <si>
+    <t>Other lodging</t>
+  </si>
+  <si>
+    <t>Utilities, fuels, and public services</t>
+  </si>
+  <si>
+    <t>Household operations</t>
+  </si>
+  <si>
+    <t>Housekeeping supplies</t>
+  </si>
+  <si>
+    <t>Household furnishings and equipment</t>
+  </si>
+  <si>
+    <t>Apparel and services</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Vehicle purchases (net outlay)</t>
+  </si>
+  <si>
+    <t>Gasoline, other fuels, and motor oil</t>
+  </si>
+  <si>
+    <t>Other vehicle expenses</t>
+  </si>
+  <si>
+    <t>Public and other transportation</t>
+  </si>
+  <si>
+    <t>Healthcare</t>
+  </si>
+  <si>
+    <t>Entertainment</t>
+  </si>
+  <si>
+    <t>Personal care products and services</t>
+  </si>
+  <si>
+    <t>Reading</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Tobacco products and smoking supplies</t>
+  </si>
+  <si>
+    <t>Miscellaneous</t>
+  </si>
+  <si>
+    <t>Cash contributions</t>
+  </si>
+  <si>
+    <t>Personal insurance and pensions</t>
+  </si>
+  <si>
+    <t>Life and other personal insurance</t>
+  </si>
+  <si>
+    <t>Pensions and Social Security</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -302,10 +443,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -621,23 +764,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81B2E13A-A86E-4147-9A8B-07F7836F86E0}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D80" sqref="D80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -660,7 +803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -677,7 +820,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -694,7 +837,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -711,7 +854,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -728,7 +871,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -745,7 +888,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -762,7 +905,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -779,7 +922,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -799,7 +942,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -816,7 +959,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -833,7 +976,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -850,7 +993,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -867,7 +1010,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -887,7 +1030,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -904,7 +1047,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -921,7 +1064,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -938,7 +1081,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -958,7 +1101,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -975,7 +1118,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -992,7 +1135,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -1009,7 +1152,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1026,7 +1169,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1043,7 +1186,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -1060,7 +1203,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -1077,7 +1220,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -1094,7 +1237,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -1111,7 +1254,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>44</v>
       </c>
@@ -1128,7 +1271,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -1145,7 +1288,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1162,7 +1305,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -1179,7 +1322,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -1196,7 +1339,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -1213,7 +1356,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -1230,7 +1373,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>51</v>
       </c>
@@ -1247,7 +1390,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -1264,7 +1407,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>53</v>
       </c>
@@ -1281,7 +1424,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -1298,7 +1441,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -1315,7 +1458,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>56</v>
       </c>
@@ -1332,7 +1475,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>57</v>
       </c>
@@ -1349,7 +1492,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -1366,7 +1509,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>59</v>
       </c>
@@ -1383,7 +1526,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>60</v>
       </c>
@@ -1400,7 +1543,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>70</v>
       </c>
@@ -1417,7 +1560,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>70</v>
       </c>
@@ -1434,7 +1577,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>70</v>
       </c>
@@ -1451,7 +1594,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>70</v>
       </c>
@@ -1466,6 +1609,507 @@
       </c>
       <c r="F48" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="3">
+        <v>6337</v>
+      </c>
+      <c r="E49" t="s">
+        <v>72</v>
+      </c>
+      <c r="F49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>77</v>
+      </c>
+      <c r="B50" t="s">
+        <v>78</v>
+      </c>
+      <c r="D50" s="4">
+        <v>85107</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51">
+        <v>49.8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>80</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D52">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>81</v>
+      </c>
+      <c r="B53" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>82</v>
+      </c>
+      <c r="B54" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>83</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>84</v>
+      </c>
+      <c r="B56" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>85</v>
+      </c>
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+      <c r="D57">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>86</v>
+      </c>
+      <c r="B58" t="s">
+        <v>78</v>
+      </c>
+      <c r="D58" s="4">
+        <v>66704</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>87</v>
+      </c>
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="D59">
+        <v>8571</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>88</v>
+      </c>
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60">
+        <v>4742</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>89</v>
+      </c>
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="D61">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>90</v>
+      </c>
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>91</v>
+      </c>
+      <c r="B63" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>92</v>
+      </c>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64">
+        <v>958</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>93</v>
+      </c>
+      <c r="B65" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>94</v>
+      </c>
+      <c r="B66" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66">
+        <v>3829</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>95</v>
+      </c>
+      <c r="B67" t="s">
+        <v>8</v>
+      </c>
+      <c r="D67">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>96</v>
+      </c>
+      <c r="B68" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68">
+        <v>22612</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>97</v>
+      </c>
+      <c r="B69" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69">
+        <v>14210</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>98</v>
+      </c>
+      <c r="B70" t="s">
+        <v>8</v>
+      </c>
+      <c r="D70">
+        <v>7514</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>99</v>
+      </c>
+      <c r="B71" t="s">
+        <v>8</v>
+      </c>
+      <c r="D71">
+        <v>5845</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>100</v>
+      </c>
+      <c r="B72" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>101</v>
+      </c>
+      <c r="B73" t="s">
+        <v>8</v>
+      </c>
+      <c r="D73">
+        <v>3847</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>102</v>
+      </c>
+      <c r="B74" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74">
+        <v>1565</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>103</v>
+      </c>
+      <c r="B75" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>104</v>
+      </c>
+      <c r="B76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76">
+        <v>2203</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>105</v>
+      </c>
+      <c r="B77" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77">
+        <v>2054</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>106</v>
+      </c>
+      <c r="B78" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78">
+        <v>10217</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>107</v>
+      </c>
+      <c r="B79" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79">
+        <v>4170</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>108</v>
+      </c>
+      <c r="B80" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80">
+        <v>2180</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>109</v>
+      </c>
+      <c r="B81" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81">
+        <v>3004</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>110</v>
+      </c>
+      <c r="B82" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>111</v>
+      </c>
+      <c r="B83" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83">
+        <v>4857</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>112</v>
+      </c>
+      <c r="B84" t="s">
+        <v>8</v>
+      </c>
+      <c r="D84">
+        <v>3540</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>113</v>
+      </c>
+      <c r="B85" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>114</v>
+      </c>
+      <c r="B86" t="s">
+        <v>8</v>
+      </c>
+      <c r="D86">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>115</v>
+      </c>
+      <c r="B87" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>116</v>
+      </c>
+      <c r="B88" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>117</v>
+      </c>
+      <c r="B89" t="s">
+        <v>8</v>
+      </c>
+      <c r="D89">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>118</v>
+      </c>
+      <c r="B90" t="s">
+        <v>8</v>
+      </c>
+      <c r="D90">
+        <v>2268</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>119</v>
+      </c>
+      <c r="B91" t="s">
+        <v>8</v>
+      </c>
+      <c r="D91">
+        <v>7882</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>120</v>
+      </c>
+      <c r="B92" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>121</v>
+      </c>
+      <c r="B93" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93">
+        <v>7560</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dictionary done for original docs
</commit_message>
<xml_diff>
--- a/data_dictionary.xlsx
+++ b/data_dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\mgsc410\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC690D27-8C7A-4DA6-BEE7-D6D0AD75698B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3DC291-A7E8-40D1-8DAE-843535359CD0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12456" yWindow="4272" windowWidth="17280" windowHeight="8964" xr2:uid="{1F7D180B-2BA4-4832-A9A8-DAB502E467AA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1F7D180B-2BA4-4832-A9A8-DAB502E467AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="123">
   <si>
     <t>Term</t>
   </si>
@@ -396,6 +397,9 @@
   </si>
   <si>
     <t>Pensions and Social Security</t>
+  </si>
+  <si>
+    <t>"midwest.xlsx""northeast.xlsx""west.xlsx""south.xlsx"</t>
   </si>
 </sst>
 </file>
@@ -766,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81B2E13A-A86E-4147-9A8B-07F7836F86E0}">
   <dimension ref="A1:G93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -776,7 +780,7 @@
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="73.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1625,7 +1629,7 @@
         <v>72</v>
       </c>
       <c r="F49" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -1638,6 +1642,12 @@
       <c r="D50" s="4">
         <v>85107</v>
       </c>
+      <c r="E50" t="s">
+        <v>72</v>
+      </c>
+      <c r="F50" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
@@ -1649,6 +1659,12 @@
       <c r="D51">
         <v>49.8</v>
       </c>
+      <c r="E51" t="s">
+        <v>72</v>
+      </c>
+      <c r="F51" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
@@ -1660,6 +1676,12 @@
       <c r="D52">
         <v>2.7</v>
       </c>
+      <c r="E52" t="s">
+        <v>72</v>
+      </c>
+      <c r="F52" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
@@ -1671,6 +1693,12 @@
       <c r="D53">
         <v>0.7</v>
       </c>
+      <c r="E53" t="s">
+        <v>72</v>
+      </c>
+      <c r="F53" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
@@ -1682,6 +1710,12 @@
       <c r="D54">
         <v>0.4</v>
       </c>
+      <c r="E54" t="s">
+        <v>72</v>
+      </c>
+      <c r="F54" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
@@ -1693,6 +1727,12 @@
       <c r="D55">
         <v>1.4</v>
       </c>
+      <c r="E55" t="s">
+        <v>72</v>
+      </c>
+      <c r="F55" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
@@ -1704,6 +1744,12 @@
       <c r="D56">
         <v>2.1</v>
       </c>
+      <c r="E56" t="s">
+        <v>72</v>
+      </c>
+      <c r="F56" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
@@ -1715,6 +1761,12 @@
       <c r="D57">
         <v>58</v>
       </c>
+      <c r="E57" t="s">
+        <v>72</v>
+      </c>
+      <c r="F57" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
@@ -1726,6 +1778,12 @@
       <c r="D58" s="4">
         <v>66704</v>
       </c>
+      <c r="E58" t="s">
+        <v>72</v>
+      </c>
+      <c r="F58" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
@@ -1737,6 +1795,12 @@
       <c r="D59">
         <v>8571</v>
       </c>
+      <c r="E59" t="s">
+        <v>72</v>
+      </c>
+      <c r="F59" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
@@ -1748,6 +1812,12 @@
       <c r="D60">
         <v>4742</v>
       </c>
+      <c r="E60" t="s">
+        <v>72</v>
+      </c>
+      <c r="F60" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
@@ -1759,6 +1829,12 @@
       <c r="D61">
         <v>596</v>
       </c>
+      <c r="E61" t="s">
+        <v>72</v>
+      </c>
+      <c r="F61" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
@@ -1770,6 +1846,12 @@
       <c r="D62">
         <v>1008</v>
       </c>
+      <c r="E62" t="s">
+        <v>72</v>
+      </c>
+      <c r="F62" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
@@ -1781,6 +1863,12 @@
       <c r="D63">
         <v>486</v>
       </c>
+      <c r="E63" t="s">
+        <v>72</v>
+      </c>
+      <c r="F63" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
@@ -1792,8 +1880,14 @@
       <c r="D64">
         <v>958</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E64" t="s">
+        <v>72</v>
+      </c>
+      <c r="F64" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>93</v>
       </c>
@@ -1803,8 +1897,14 @@
       <c r="D65">
         <v>1694</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E65" t="s">
+        <v>72</v>
+      </c>
+      <c r="F65" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>94</v>
       </c>
@@ -1814,8 +1914,14 @@
       <c r="D66">
         <v>3829</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E66" t="s">
+        <v>72</v>
+      </c>
+      <c r="F66" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>95</v>
       </c>
@@ -1825,8 +1931,14 @@
       <c r="D67">
         <v>663</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E67" t="s">
+        <v>72</v>
+      </c>
+      <c r="F67" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>96</v>
       </c>
@@ -1836,8 +1948,14 @@
       <c r="D68">
         <v>22612</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E68" t="s">
+        <v>72</v>
+      </c>
+      <c r="F68" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>97</v>
       </c>
@@ -1847,8 +1965,14 @@
       <c r="D69">
         <v>14210</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E69" t="s">
+        <v>72</v>
+      </c>
+      <c r="F69" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>98</v>
       </c>
@@ -1858,8 +1982,14 @@
       <c r="D70">
         <v>7514</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E70" t="s">
+        <v>72</v>
+      </c>
+      <c r="F70" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>99</v>
       </c>
@@ -1869,8 +1999,14 @@
       <c r="D71">
         <v>5845</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E71" t="s">
+        <v>72</v>
+      </c>
+      <c r="F71" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>100</v>
       </c>
@@ -1880,8 +2016,14 @@
       <c r="D72">
         <v>851</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E72" t="s">
+        <v>72</v>
+      </c>
+      <c r="F72" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>101</v>
       </c>
@@ -1891,8 +2033,14 @@
       <c r="D73">
         <v>3847</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E73" t="s">
+        <v>72</v>
+      </c>
+      <c r="F73" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>102</v>
       </c>
@@ -1902,8 +2050,14 @@
       <c r="D74">
         <v>1565</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E74" t="s">
+        <v>72</v>
+      </c>
+      <c r="F74" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>103</v>
       </c>
@@ -1913,8 +2067,14 @@
       <c r="D75">
         <v>788</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E75" t="s">
+        <v>72</v>
+      </c>
+      <c r="F75" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>104</v>
       </c>
@@ -1924,8 +2084,14 @@
       <c r="D76">
         <v>2203</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E76" t="s">
+        <v>72</v>
+      </c>
+      <c r="F76" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>105</v>
       </c>
@@ -1935,8 +2101,14 @@
       <c r="D77">
         <v>2054</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E77" t="s">
+        <v>72</v>
+      </c>
+      <c r="F77" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>106</v>
       </c>
@@ -1946,8 +2118,14 @@
       <c r="D78">
         <v>10217</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E78" t="s">
+        <v>72</v>
+      </c>
+      <c r="F78" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>107</v>
       </c>
@@ -1957,8 +2135,14 @@
       <c r="D79">
         <v>4170</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E79" t="s">
+        <v>72</v>
+      </c>
+      <c r="F79" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>108</v>
       </c>
@@ -1968,8 +2152,14 @@
       <c r="D80">
         <v>2180</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E80" t="s">
+        <v>72</v>
+      </c>
+      <c r="F80" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>109</v>
       </c>
@@ -1979,8 +2169,14 @@
       <c r="D81">
         <v>3004</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E81" t="s">
+        <v>72</v>
+      </c>
+      <c r="F81" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>110</v>
       </c>
@@ -1990,8 +2186,14 @@
       <c r="D82">
         <v>863</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E82" t="s">
+        <v>72</v>
+      </c>
+      <c r="F82" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>111</v>
       </c>
@@ -2001,8 +2203,14 @@
       <c r="D83">
         <v>4857</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E83" t="s">
+        <v>72</v>
+      </c>
+      <c r="F83" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>112</v>
       </c>
@@ -2012,8 +2220,14 @@
       <c r="D84">
         <v>3540</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E84" t="s">
+        <v>72</v>
+      </c>
+      <c r="F84" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>113</v>
       </c>
@@ -2023,8 +2237,14 @@
       <c r="D85">
         <v>854</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E85" t="s">
+        <v>72</v>
+      </c>
+      <c r="F85" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>114</v>
       </c>
@@ -2034,8 +2254,14 @@
       <c r="D86">
         <v>143</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E86" t="s">
+        <v>72</v>
+      </c>
+      <c r="F86" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>115</v>
       </c>
@@ -2045,8 +2271,14 @@
       <c r="D87">
         <v>1518</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E87" t="s">
+        <v>72</v>
+      </c>
+      <c r="F87" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>116</v>
       </c>
@@ -2056,8 +2288,14 @@
       <c r="D88">
         <v>249</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E88" t="s">
+        <v>72</v>
+      </c>
+      <c r="F88" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>117</v>
       </c>
@@ -2067,8 +2305,14 @@
       <c r="D89">
         <v>1275</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E89" t="s">
+        <v>72</v>
+      </c>
+      <c r="F89" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>118</v>
       </c>
@@ -2078,8 +2322,14 @@
       <c r="D90">
         <v>2268</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E90" t="s">
+        <v>72</v>
+      </c>
+      <c r="F90" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>119</v>
       </c>
@@ -2089,8 +2339,14 @@
       <c r="D91">
         <v>7882</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E91" t="s">
+        <v>72</v>
+      </c>
+      <c r="F91" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>120</v>
       </c>
@@ -2100,8 +2356,14 @@
       <c r="D92">
         <v>322</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E92" t="s">
+        <v>72</v>
+      </c>
+      <c r="F92" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>121</v>
       </c>
@@ -2110,6 +2372,12 @@
       </c>
       <c r="D93">
         <v>7560</v>
+      </c>
+      <c r="E93" t="s">
+        <v>72</v>
+      </c>
+      <c r="F93" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>